<commit_message>
update BH thang 4
</commit_message>
<xml_diff>
--- a/5. WS/1. Bộ phận bảo hành/1. Thực hiện sửa chữa bảo hành/nam2023/Thang3/2.XuLyBH/XLBH2303_KimLong.xlsx
+++ b/5. WS/1. Bộ phận bảo hành/1. Thực hiện sửa chữa bảo hành/nam2023/Thang3/2.XuLyBH/XLBH2303_KimLong.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\PhongBaoHanh\VNET\5. WS\1. Bộ phận bảo hành\1. Thực hiện sửa chữa bảo hành\nam2023\Thang3\2.XuLyBH\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VNET\5. WS\1. Bộ phận bảo hành\1. Thực hiện sửa chữa bảo hành\nam2023\Thang3\2.XuLyBH\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="72">
   <si>
     <t>STT</t>
   </si>
@@ -225,7 +225,28 @@
     <t>Kim Long</t>
   </si>
   <si>
-    <t>Không check được</t>
+    <t>1205220010</t>
+  </si>
+  <si>
+    <t>Thiết bị không nhận nhiệt độ</t>
+  </si>
+  <si>
+    <t>Thay IC giap tiếp, xử lý lại main</t>
+  </si>
+  <si>
+    <t>Tùng</t>
+  </si>
+  <si>
+    <t>2111048</t>
+  </si>
+  <si>
+    <t>Thiết bị hoạt động bình thường</t>
+  </si>
+  <si>
+    <t>Test lại thiết bị</t>
+  </si>
+  <si>
+    <t>Mất ID</t>
   </si>
 </sst>
 </file>
@@ -428,7 +449,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -644,6 +665,33 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -953,7 +1001,7 @@
   <dimension ref="A1:X115"/>
   <sheetViews>
     <sheetView showZeros="0" tabSelected="1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:B8"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1149,32 +1197,44 @@
       <c r="A6" s="3">
         <v>1</v>
       </c>
-      <c r="B6" s="47">
-        <v>45007</v>
-      </c>
-      <c r="C6" s="47"/>
-      <c r="D6" s="31" t="s">
+      <c r="B6" s="73">
+        <v>45013</v>
+      </c>
+      <c r="C6" s="73">
+        <v>45015</v>
+      </c>
+      <c r="D6" s="46" t="s">
         <v>57</v>
       </c>
-      <c r="E6" s="32">
-        <v>1205220010</v>
-      </c>
-      <c r="F6" s="39"/>
-      <c r="G6" s="31" t="s">
+      <c r="E6" s="74" t="s">
+        <v>64</v>
+      </c>
+      <c r="F6" s="46"/>
+      <c r="G6" s="46" t="s">
         <v>62</v>
       </c>
-      <c r="H6" s="48"/>
-      <c r="I6" s="49"/>
-      <c r="J6" s="50"/>
-      <c r="K6" s="51"/>
-      <c r="L6" s="51"/>
-      <c r="M6" s="52"/>
-      <c r="N6" s="50"/>
-      <c r="O6" s="50"/>
-      <c r="P6" s="52"/>
-      <c r="Q6" s="50"/>
-      <c r="R6" s="53"/>
-      <c r="S6" s="55"/>
+      <c r="H6" s="46"/>
+      <c r="I6" s="75"/>
+      <c r="J6" s="76" t="s">
+        <v>65</v>
+      </c>
+      <c r="K6" s="77"/>
+      <c r="L6" s="78"/>
+      <c r="M6" s="78" t="s">
+        <v>66</v>
+      </c>
+      <c r="N6" s="76"/>
+      <c r="O6" s="76"/>
+      <c r="P6" s="78" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q6" s="76" t="s">
+        <v>18</v>
+      </c>
+      <c r="R6" s="79" t="s">
+        <v>30</v>
+      </c>
+      <c r="S6" s="80"/>
       <c r="T6" s="12"/>
       <c r="U6" s="66" t="s">
         <v>18</v>
@@ -1188,32 +1248,44 @@
       <c r="A7" s="3">
         <v>2</v>
       </c>
-      <c r="B7" s="47">
-        <v>45007</v>
-      </c>
-      <c r="C7" s="47"/>
-      <c r="D7" s="31" t="s">
+      <c r="B7" s="73">
+        <v>45013</v>
+      </c>
+      <c r="C7" s="73">
+        <v>45015</v>
+      </c>
+      <c r="D7" s="46" t="s">
         <v>57</v>
       </c>
-      <c r="E7" s="32" t="s">
-        <v>64</v>
-      </c>
-      <c r="F7" s="39"/>
-      <c r="G7" s="31" t="s">
+      <c r="E7" s="74" t="s">
+        <v>68</v>
+      </c>
+      <c r="F7" s="46"/>
+      <c r="G7" s="46" t="s">
         <v>62</v>
       </c>
-      <c r="H7" s="48"/>
-      <c r="I7" s="49"/>
-      <c r="J7" s="50"/>
-      <c r="K7" s="51"/>
-      <c r="L7" s="51"/>
-      <c r="M7" s="52"/>
-      <c r="N7" s="50"/>
-      <c r="O7" s="50"/>
-      <c r="P7" s="52"/>
-      <c r="Q7" s="50"/>
-      <c r="R7" s="53"/>
-      <c r="S7" s="55"/>
+      <c r="H7" s="46"/>
+      <c r="I7" s="75"/>
+      <c r="J7" s="76" t="s">
+        <v>65</v>
+      </c>
+      <c r="K7" s="77"/>
+      <c r="L7" s="77"/>
+      <c r="M7" s="78" t="s">
+        <v>66</v>
+      </c>
+      <c r="N7" s="76"/>
+      <c r="O7" s="76"/>
+      <c r="P7" s="78" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q7" s="76" t="s">
+        <v>18</v>
+      </c>
+      <c r="R7" s="79" t="s">
+        <v>30</v>
+      </c>
+      <c r="S7" s="80"/>
       <c r="T7" s="12"/>
       <c r="U7" s="67"/>
       <c r="V7" s="3" t="s">
@@ -1225,32 +1297,44 @@
       <c r="A8" s="3">
         <v>3</v>
       </c>
-      <c r="B8" s="47">
-        <v>45007</v>
-      </c>
-      <c r="C8" s="47"/>
-      <c r="D8" s="31" t="s">
+      <c r="B8" s="73">
+        <v>45013</v>
+      </c>
+      <c r="C8" s="73">
+        <v>45015</v>
+      </c>
+      <c r="D8" s="46" t="s">
         <v>57</v>
       </c>
-      <c r="E8" s="32" t="s">
-        <v>64</v>
+      <c r="E8" s="81">
+        <v>2111045</v>
       </c>
       <c r="F8" s="46"/>
-      <c r="G8" s="31" t="s">
+      <c r="G8" s="46" t="s">
         <v>62</v>
       </c>
-      <c r="H8" s="48"/>
-      <c r="I8" s="49"/>
-      <c r="J8" s="50"/>
-      <c r="K8" s="51"/>
-      <c r="L8" s="52"/>
-      <c r="M8" s="52"/>
-      <c r="N8" s="50"/>
-      <c r="O8" s="50"/>
-      <c r="P8" s="52"/>
-      <c r="Q8" s="50"/>
-      <c r="R8" s="53"/>
-      <c r="S8" s="55"/>
+      <c r="H8" s="46"/>
+      <c r="I8" s="75"/>
+      <c r="J8" s="76" t="s">
+        <v>69</v>
+      </c>
+      <c r="K8" s="77"/>
+      <c r="L8" s="77"/>
+      <c r="M8" s="78" t="s">
+        <v>70</v>
+      </c>
+      <c r="N8" s="76"/>
+      <c r="O8" s="76"/>
+      <c r="P8" s="78" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q8" s="76" t="s">
+        <v>19</v>
+      </c>
+      <c r="R8" s="79" t="s">
+        <v>25</v>
+      </c>
+      <c r="S8" s="80"/>
       <c r="T8" s="12"/>
       <c r="U8" s="67"/>
       <c r="V8" s="3" t="s">
@@ -1262,24 +1346,44 @@
       <c r="A9" s="3">
         <v>4</v>
       </c>
-      <c r="B9" s="47"/>
-      <c r="C9" s="47"/>
-      <c r="D9" s="48"/>
-      <c r="E9" s="54"/>
-      <c r="F9" s="57"/>
-      <c r="G9" s="48"/>
-      <c r="H9" s="48"/>
-      <c r="I9" s="49"/>
-      <c r="J9" s="50"/>
-      <c r="K9" s="51"/>
-      <c r="L9" s="51"/>
-      <c r="M9" s="52"/>
-      <c r="N9" s="50"/>
-      <c r="O9" s="50"/>
-      <c r="P9" s="52"/>
-      <c r="Q9" s="50"/>
-      <c r="R9" s="53"/>
-      <c r="S9" s="55"/>
+      <c r="B9" s="73">
+        <v>45013</v>
+      </c>
+      <c r="C9" s="73">
+        <v>45015</v>
+      </c>
+      <c r="D9" s="46" t="s">
+        <v>57</v>
+      </c>
+      <c r="E9" s="81" t="s">
+        <v>71</v>
+      </c>
+      <c r="F9" s="46"/>
+      <c r="G9" s="46" t="s">
+        <v>62</v>
+      </c>
+      <c r="H9" s="46"/>
+      <c r="I9" s="75"/>
+      <c r="J9" s="76" t="s">
+        <v>65</v>
+      </c>
+      <c r="K9" s="76"/>
+      <c r="L9" s="77"/>
+      <c r="M9" s="78" t="s">
+        <v>66</v>
+      </c>
+      <c r="N9" s="76"/>
+      <c r="O9" s="76"/>
+      <c r="P9" s="78" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q9" s="76" t="s">
+        <v>18</v>
+      </c>
+      <c r="R9" s="79" t="s">
+        <v>30</v>
+      </c>
+      <c r="S9" s="80"/>
       <c r="T9" s="12"/>
       <c r="U9" s="67"/>
       <c r="V9" s="3" t="s">
@@ -1291,24 +1395,44 @@
       <c r="A10" s="3">
         <v>5</v>
       </c>
-      <c r="B10" s="47"/>
-      <c r="C10" s="47"/>
-      <c r="D10" s="48"/>
-      <c r="E10" s="54"/>
-      <c r="F10" s="57"/>
-      <c r="G10" s="48"/>
-      <c r="H10" s="48"/>
-      <c r="I10" s="49"/>
-      <c r="J10" s="50"/>
-      <c r="K10" s="54"/>
-      <c r="L10" s="51"/>
-      <c r="M10" s="52"/>
-      <c r="N10" s="50"/>
-      <c r="O10" s="50"/>
-      <c r="P10" s="52"/>
-      <c r="Q10" s="50"/>
-      <c r="R10" s="53"/>
-      <c r="S10" s="55"/>
+      <c r="B10" s="73">
+        <v>45013</v>
+      </c>
+      <c r="C10" s="73">
+        <v>45015</v>
+      </c>
+      <c r="D10" s="46" t="s">
+        <v>57</v>
+      </c>
+      <c r="E10" s="81" t="s">
+        <v>71</v>
+      </c>
+      <c r="F10" s="46"/>
+      <c r="G10" s="46" t="s">
+        <v>62</v>
+      </c>
+      <c r="H10" s="46"/>
+      <c r="I10" s="75"/>
+      <c r="J10" s="76" t="s">
+        <v>65</v>
+      </c>
+      <c r="K10" s="81"/>
+      <c r="L10" s="78"/>
+      <c r="M10" s="78" t="s">
+        <v>66</v>
+      </c>
+      <c r="N10" s="76"/>
+      <c r="O10" s="76"/>
+      <c r="P10" s="78" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q10" s="76" t="s">
+        <v>18</v>
+      </c>
+      <c r="R10" s="79" t="s">
+        <v>30</v>
+      </c>
+      <c r="S10" s="80"/>
       <c r="T10" s="12"/>
       <c r="U10" s="67"/>
       <c r="V10" s="3" t="s">
@@ -1636,7 +1760,7 @@
       </c>
       <c r="V21" s="3">
         <f>COUNTIF($Q$6:$Q$51,"PC")</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="W21" s="12"/>
     </row>
@@ -3187,6 +3311,13 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="U6:U11"/>
+    <mergeCell ref="U12:U16"/>
+    <mergeCell ref="P4:P5"/>
+    <mergeCell ref="Q4:Q5"/>
+    <mergeCell ref="R4:R5"/>
+    <mergeCell ref="S4:S5"/>
+    <mergeCell ref="U4:U5"/>
     <mergeCell ref="V4:V5"/>
     <mergeCell ref="A1:V1"/>
     <mergeCell ref="A2:D2"/>
@@ -3198,13 +3329,6 @@
     <mergeCell ref="M4:M5"/>
     <mergeCell ref="N4:N5"/>
     <mergeCell ref="O4:O5"/>
-    <mergeCell ref="U6:U11"/>
-    <mergeCell ref="U12:U16"/>
-    <mergeCell ref="P4:P5"/>
-    <mergeCell ref="Q4:Q5"/>
-    <mergeCell ref="R4:R5"/>
-    <mergeCell ref="S4:S5"/>
-    <mergeCell ref="U4:U5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4956,13 +5080,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="U6:U11"/>
-    <mergeCell ref="U12:U16"/>
-    <mergeCell ref="P4:P5"/>
-    <mergeCell ref="Q4:Q5"/>
-    <mergeCell ref="R4:R5"/>
-    <mergeCell ref="S4:S5"/>
-    <mergeCell ref="U4:U5"/>
     <mergeCell ref="V4:V5"/>
     <mergeCell ref="A1:V1"/>
     <mergeCell ref="A2:D2"/>
@@ -4974,6 +5091,13 @@
     <mergeCell ref="M4:M5"/>
     <mergeCell ref="N4:N5"/>
     <mergeCell ref="O4:O5"/>
+    <mergeCell ref="U6:U11"/>
+    <mergeCell ref="U12:U16"/>
+    <mergeCell ref="P4:P5"/>
+    <mergeCell ref="Q4:Q5"/>
+    <mergeCell ref="R4:R5"/>
+    <mergeCell ref="S4:S5"/>
+    <mergeCell ref="U4:U5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>